<commit_message>
DAC Connected to FPGA TX Bus init commit TX STM32 init commit
</commit_message>
<xml_diff>
--- a/Scheme/Smeta.xlsx
+++ b/Scheme/Smeta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Наименование</t>
   </si>
@@ -192,6 +192,21 @@
   </si>
   <si>
     <t>https://ru.aliexpress.com/item/RS485-communication-module-sound-detector-sound-level-scoring-shell-instrument-noise-sensor-WST60M/32827169756.html</t>
+  </si>
+  <si>
+    <t>Плата ЦАП</t>
+  </si>
+  <si>
+    <t>DAC904E</t>
+  </si>
+  <si>
+    <t>https://ru.aliexpress.com/item/DAC904E-DAC902E-DAC900E-DAC908E-2-SMD/32864490960.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Резистор 2к 0805 </t>
+  </si>
+  <si>
+    <t>Конденсатор 1мкф</t>
   </si>
 </sst>
 </file>
@@ -569,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F49"/>
+  <dimension ref="B2:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +651,7 @@
         <v>182.11</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" ref="E5:E47" si="0">C5*D5</f>
+        <f t="shared" ref="E5:E55" si="0">C5*D5</f>
         <v>182.11</v>
       </c>
     </row>
@@ -790,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
@@ -806,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
@@ -822,417 +837,534 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
       </c>
       <c r="D20" s="7">
-        <v>145</v>
+        <v>67.5</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+        <v>67.5</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="7">
+        <f>C21*D21</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
       </c>
       <c r="D22" s="7">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
       </c>
       <c r="D23" s="7">
-        <v>17</v>
+        <f>7/5</f>
+        <v>1.4</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C24" s="5">
         <v>2</v>
       </c>
       <c r="D24" s="7">
-        <v>17</v>
-      </c>
-      <c r="E24" s="7">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="5">
-        <v>5</v>
-      </c>
-      <c r="D26" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
-      <c r="E26" s="7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="5">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7">
-        <v>6</v>
-      </c>
-      <c r="E27" s="7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="5">
-        <v>1</v>
-      </c>
-      <c r="D28" s="7">
-        <v>12</v>
-      </c>
-      <c r="E28" s="7">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="E24" s="7">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="5">
         <v>4</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D25" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
-      <c r="E29" s="7">
-        <f t="shared" si="0"/>
+      <c r="E25" s="7">
+        <f>C25*D25</f>
         <v>5.6</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="5">
+        <v>2</v>
+      </c>
+      <c r="D26" s="7">
+        <v>6</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
+        <v>145</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7">
+        <v>17</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7">
+        <v>17</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="5">
         <v>2</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D32" s="7">
+        <v>17</v>
+      </c>
+      <c r="E32" s="7">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="5">
+        <v>5</v>
+      </c>
+      <c r="D34" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E34" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="7">
+        <v>6</v>
+      </c>
+      <c r="E35" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7">
+        <v>12</v>
+      </c>
+      <c r="E36" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="5">
+        <v>4</v>
+      </c>
+      <c r="D37" s="7">
+        <f>7/5</f>
+        <v>1.4</v>
+      </c>
+      <c r="E37" s="7">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="5">
+        <v>2</v>
+      </c>
+      <c r="D38" s="7">
+        <f>7/5</f>
+        <v>1.4</v>
+      </c>
+      <c r="E38" s="7">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C39" s="5">
         <v>2</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D39" s="7">
         <v>0.9</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E39" s="7">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="5">
-        <v>1</v>
-      </c>
-      <c r="D32" s="7">
+      <c r="C40" s="5">
+        <v>1</v>
+      </c>
+      <c r="D40" s="7">
         <f>5/10</f>
         <v>0.5</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E40" s="7">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="5">
-        <v>1</v>
-      </c>
-      <c r="D33" s="7">
+      <c r="C41" s="5">
+        <v>1</v>
+      </c>
+      <c r="D41" s="7">
         <f>5/10</f>
         <v>0.5</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E41" s="7">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="5">
-        <v>1</v>
-      </c>
-      <c r="D34" s="7">
+      <c r="C42" s="5">
+        <v>1</v>
+      </c>
+      <c r="D42" s="7">
         <v>0.9</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E42" s="7">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="5">
-        <v>1</v>
-      </c>
-      <c r="D35" s="7">
+      <c r="C43" s="5">
+        <v>1</v>
+      </c>
+      <c r="D43" s="7">
         <f>5/10</f>
         <v>0.5</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E43" s="7">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="5">
-        <v>1</v>
-      </c>
-      <c r="D36" s="7">
+      <c r="C44" s="5">
+        <v>1</v>
+      </c>
+      <c r="D44" s="7">
         <f>5/10</f>
         <v>0.5</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E44" s="7">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C45" s="5">
         <v>3</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D45" s="7">
         <f>5/10</f>
         <v>0.5</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E45" s="7">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="5">
-        <v>1</v>
-      </c>
-      <c r="D38" s="7">
+      <c r="C46" s="5">
+        <v>1</v>
+      </c>
+      <c r="D46" s="7">
         <v>8</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E46" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="5">
-        <v>1</v>
-      </c>
-      <c r="D39" s="7">
+      <c r="C47" s="5">
+        <v>1</v>
+      </c>
+      <c r="D47" s="7">
         <v>4</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E47" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="5">
-        <v>1</v>
-      </c>
-      <c r="D40" s="7">
+      <c r="C48" s="5">
+        <v>1</v>
+      </c>
+      <c r="D48" s="7">
         <f>129.2/10</f>
         <v>12.919999999999998</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E48" s="7">
         <f t="shared" si="0"/>
         <v>12.919999999999998</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C49" s="5">
         <v>2</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D49" s="7">
         <v>11</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E49" s="7">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C50" s="5">
         <v>4</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D50" s="7">
         <v>6</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E50" s="7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="5">
-        <v>1</v>
-      </c>
-      <c r="D43" s="7">
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+      <c r="D51" s="7">
         <v>150</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E51" s="7">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="5">
-        <v>1</v>
-      </c>
-      <c r="D44" s="7">
+      <c r="C52" s="5">
+        <v>1</v>
+      </c>
+      <c r="D52" s="7">
         <v>4</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E52" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="5">
-        <v>1</v>
-      </c>
-      <c r="D45" s="7">
+      <c r="C53" s="5">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7">
         <v>46</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E53" s="7">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="3" t="s">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="5">
-        <v>1</v>
-      </c>
-      <c r="D47" s="7">
+      <c r="C55" s="5">
+        <v>1</v>
+      </c>
+      <c r="D55" s="7">
         <v>79</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E55" s="7">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="8" t="s">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="8">
-        <f>SUM(E3:E48)</f>
-        <v>7241.08</v>
+      <c r="E57" s="8">
+        <f>SUM(E3:E56)</f>
+        <v>7335.88</v>
       </c>
     </row>
   </sheetData>
@@ -1243,8 +1375,9 @@
     <hyperlink ref="F4" r:id="rId4"/>
     <hyperlink ref="F12" r:id="rId5"/>
     <hyperlink ref="F14" r:id="rId6"/>
+    <hyperlink ref="F20" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FFT Optimize Menu navigation buttons Freq selecton by touchpad TX-RX relay New optical Encoder 600pos Dedicated PLL_3
</commit_message>
<xml_diff>
--- a/Scheme/Smeta.xlsx
+++ b/Scheme/Smeta.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>Наименование</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Питание</t>
   </si>
   <si>
-    <t>Плата предусилителя</t>
-  </si>
-  <si>
     <t>Транзистор BFG591</t>
   </si>
   <si>
@@ -98,12 +95,6 @@
     <t>Модуль PAM8403 ADJ УНЧ 2*3W 2,5-5V с регулятором</t>
   </si>
   <si>
-    <t>7812 TO220 12V 1,5A (КР142ЕН8Б)</t>
-  </si>
-  <si>
-    <t>7805 TO220 5V 1,5A (КР142ЕН5А)</t>
-  </si>
-  <si>
     <t>Стабилизатор LM1117S-ADJ D2PAK</t>
   </si>
   <si>
@@ -155,18 +146,12 @@
     <t xml:space="preserve">Резистор 470ом 0805 </t>
   </si>
   <si>
-    <t>Модуль энкодера KY-040</t>
-  </si>
-  <si>
     <t>Другое</t>
   </si>
   <si>
     <t>Гнездо PL на корпус фланец</t>
   </si>
   <si>
-    <t>Конденсатор 2200мкФ 25В</t>
-  </si>
-  <si>
     <t>Трансфлюктор М30ВН-6Тр 16*9*7</t>
   </si>
   <si>
@@ -207,6 +192,57 @@
   </si>
   <si>
     <t>Конденсатор 1мкф</t>
+  </si>
+  <si>
+    <t>Корпус РЭА №15-9 200*165*65</t>
+  </si>
+  <si>
+    <t>Плата УВЧ (Preamp)</t>
+  </si>
+  <si>
+    <t>https://ru.aliexpress.com/item/Free-Shipping-1pc-Incremental-rotary-encoder-600-lines/1280677743.html</t>
+  </si>
+  <si>
+    <t>Гнездо "Банан"</t>
+  </si>
+  <si>
+    <t>Штекер MIC 8pin</t>
+  </si>
+  <si>
+    <t>Кварц 12МГц HC-49US</t>
+  </si>
+  <si>
+    <t>Конденсатор 22пф</t>
+  </si>
+  <si>
+    <t>Гнездо питания 5,5*2,1</t>
+  </si>
+  <si>
+    <t>Мембранная клавиатура 1*4</t>
+  </si>
+  <si>
+    <t>Диод Шоттки SR860 (SB860) DO-201 60V 8A</t>
+  </si>
+  <si>
+    <t>DC-DC 4,0-38V -&gt; 1,25-36V 5A LM2596S-ADJ понижающий</t>
+  </si>
+  <si>
+    <t>Кнопка питания, с фиксацией PBS-16A 220М 1A</t>
+  </si>
+  <si>
+    <t>Оптический энкодер 600 позиций на оборот</t>
+  </si>
+  <si>
+    <t>Гнездо SMA на плату</t>
+  </si>
+  <si>
+    <t>Переключатель TX-RX</t>
+  </si>
+  <si>
+    <t>Модуль реле 1-канальный 5В 10A 250V/реле</t>
+  </si>
+  <si>
+    <t>SMA-SMA патч корд 6,5"</t>
   </si>
 </sst>
 </file>
@@ -584,16 +620,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F57"/>
+  <dimension ref="B2:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="5"/>
     <col min="4" max="4" width="11.28515625" style="7" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="7"/>
@@ -614,7 +650,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -637,7 +673,7 @@
         <v>2278.73</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -651,7 +687,7 @@
         <v>182.11</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" ref="E5:E55" si="0">C5*D5</f>
+        <f t="shared" ref="E5:E68" si="0">C5*D5</f>
         <v>182.11</v>
       </c>
     </row>
@@ -675,7 +711,7 @@
         <v>707.81</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -693,12 +729,12 @@
         <v>479.67</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -711,208 +747,210 @@
         <v>714.68</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
-        <v>90</v>
-      </c>
-      <c r="E10" s="7">
-        <f t="shared" si="0"/>
-        <v>90</v>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>7</v>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>933.21</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>933.21</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
       </c>
       <c r="D12" s="7">
-        <v>933.21</v>
+        <v>10</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
-        <v>933.21</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>54</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7">
+        <f>7/5</f>
+        <v>1.4</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
         <v>1236.95</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E15" s="7">
         <f t="shared" si="0"/>
         <v>1236.95</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
-        <v>12</v>
-      </c>
-      <c r="E15" s="7">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="F15" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
       </c>
       <c r="D16" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C18" s="5">
         <v>2</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D18" s="7">
         <f>5/10</f>
         <v>0.5</v>
       </c>
-      <c r="E17" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E19" s="7">
         <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="5">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7">
-        <v>67.5</v>
-      </c>
-      <c r="E20" s="7">
-        <f t="shared" si="0"/>
-        <v>67.5</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>58</v>
+      <c r="B20" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
       </c>
       <c r="D21" s="7">
+        <v>67.5</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
+        <v>67.5</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
         <f>5/10</f>
         <v>0.5</v>
       </c>
-      <c r="E21" s="7">
-        <f>C21*D21</f>
+      <c r="E22" s="7">
+        <f>C22*D22</f>
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7">
-        <v>5</v>
-      </c>
-      <c r="E22" s="7">
-        <f t="shared" si="0"/>
-        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
       </c>
       <c r="D23" s="7">
-        <f>7/5</f>
-        <v>1.4</v>
+        <v>5</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>1.4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="7">
         <f>7/5</f>
@@ -920,159 +958,160 @@
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C25" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D25" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
       <c r="E25" s="7">
-        <f>C25*D25</f>
-        <v>5.6</v>
+        <f t="shared" si="0"/>
+        <v>2.8</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C26" s="5">
+        <v>4</v>
+      </c>
+      <c r="D26" s="7">
+        <f>7/5</f>
+        <v>1.4</v>
+      </c>
+      <c r="E26" s="7">
+        <f>C26*D26</f>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="5">
         <v>2</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D27" s="7">
         <v>6</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E27" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
       </c>
       <c r="D28" s="7">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
       </c>
       <c r="D30" s="7">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="5">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7">
-        <v>17</v>
-      </c>
-      <c r="E31" s="7">
-        <f t="shared" si="0"/>
-        <v>17</v>
+      <c r="B31" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C32" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="7">
-        <v>17</v>
+        <v>170</v>
       </c>
       <c r="E32" s="7">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>17</v>
+      <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7">
+        <v>18</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="5">
+      <c r="B34" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="5">
         <v>5</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D35" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E35" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="5">
-        <v>1</v>
-      </c>
-      <c r="D35" s="7">
-        <v>6</v>
-      </c>
-      <c r="E35" s="7">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C36" s="5">
         <v>1</v>
       </c>
       <c r="D36" s="7">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E36" s="7">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -1080,23 +1119,22 @@
         <v>35</v>
       </c>
       <c r="C37" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D37" s="7">
-        <f>7/5</f>
-        <v>1.4</v>
+        <v>12</v>
       </c>
       <c r="E37" s="7">
         <f t="shared" si="0"/>
-        <v>5.6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C38" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D38" s="7">
         <f>7/5</f>
@@ -1104,43 +1142,43 @@
       </c>
       <c r="E38" s="7">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C39" s="5">
         <v>2</v>
       </c>
       <c r="D39" s="7">
-        <v>0.9</v>
+        <f>7/5</f>
+        <v>1.4</v>
       </c>
       <c r="E39" s="7">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C40" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="7">
-        <f>5/10</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E40" s="7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C41" s="5">
         <v>1</v>
@@ -1156,38 +1194,38 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C42" s="5">
         <v>1</v>
       </c>
       <c r="D42" s="7">
-        <v>0.9</v>
+        <f>5/10</f>
+        <v>0.5</v>
       </c>
       <c r="E42" s="7">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C43" s="5">
         <v>1</v>
       </c>
       <c r="D43" s="7">
-        <f>5/10</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E43" s="7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" s="5">
         <v>1</v>
@@ -1203,10 +1241,10 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C45" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D45" s="7">
         <f>5/10</f>
@@ -1214,101 +1252,102 @@
       </c>
       <c r="E45" s="7">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C46" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46" s="7">
-        <v>8</v>
+        <f>5/10</f>
+        <v>0.5</v>
       </c>
       <c r="E46" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C47" s="5">
         <v>1</v>
       </c>
       <c r="D47" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E47" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C48" s="5">
         <v>1</v>
       </c>
       <c r="D48" s="7">
+        <v>4</v>
+      </c>
+      <c r="E48" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1</v>
+      </c>
+      <c r="D49" s="7">
         <f>129.2/10</f>
         <v>12.919999999999998</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E49" s="7">
         <f t="shared" si="0"/>
         <v>12.919999999999998</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="5">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="5">
         <v>2</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D50" s="7">
         <v>11</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E50" s="7">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="5">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="5">
         <v>4</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D51" s="7">
         <v>6</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E51" s="7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" s="5">
-        <v>1</v>
-      </c>
-      <c r="D51" s="7">
-        <v>150</v>
-      </c>
-      <c r="E51" s="7">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>20</v>
       </c>
@@ -1316,55 +1355,249 @@
         <v>1</v>
       </c>
       <c r="D52" s="7">
+        <v>150</v>
+      </c>
+      <c r="E52" s="7">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="5">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7">
         <v>4</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E53" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" s="5">
-        <v>1</v>
-      </c>
-      <c r="D53" s="7">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
+      </c>
+      <c r="D54" s="7">
         <v>46</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E54" s="7">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C55" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" s="7">
         <v>79</v>
       </c>
       <c r="E55" s="7">
         <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="5">
+        <v>1</v>
+      </c>
+      <c r="D57" s="7">
+        <v>89</v>
+      </c>
+      <c r="E57" s="7">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="5">
+        <v>2</v>
+      </c>
+      <c r="D58" s="7">
         <v>79</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="8" t="s">
+      <c r="E58" s="7">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="5">
+        <v>1</v>
+      </c>
+      <c r="D60" s="7">
+        <v>79</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" s="5">
+        <v>1</v>
+      </c>
+      <c r="D61" s="7">
+        <v>525</v>
+      </c>
+      <c r="E61" s="7">
+        <f t="shared" si="0"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1</v>
+      </c>
+      <c r="D62" s="7">
+        <v>962</v>
+      </c>
+      <c r="E62" s="7">
+        <f t="shared" si="0"/>
+        <v>962</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="5">
+        <v>1</v>
+      </c>
+      <c r="D63" s="7">
+        <v>32</v>
+      </c>
+      <c r="E63" s="7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F63" s="10"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1</v>
+      </c>
+      <c r="D64" s="7">
+        <v>45</v>
+      </c>
+      <c r="E64" s="7">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F64" s="10"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="5">
+        <v>1</v>
+      </c>
+      <c r="D65" s="7">
+        <v>27</v>
+      </c>
+      <c r="E65" s="7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="F65" s="10"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="5">
+        <v>1</v>
+      </c>
+      <c r="D66" s="7">
+        <v>60</v>
+      </c>
+      <c r="E66" s="7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F66" s="10"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" s="5">
+        <v>1</v>
+      </c>
+      <c r="D67" s="7">
+        <v>35</v>
+      </c>
+      <c r="E67" s="7">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="F67" s="10"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" s="5">
+        <v>3</v>
+      </c>
+      <c r="D68" s="7">
+        <v>67</v>
+      </c>
+      <c r="E68" s="7">
+        <f t="shared" si="0"/>
+        <v>201</v>
+      </c>
+      <c r="F68" s="10"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E57" s="8">
-        <f>SUM(E3:E56)</f>
-        <v>7335.88</v>
+      <c r="E69" s="8">
+        <f>SUM(E3:E68)</f>
+        <v>9749.68</v>
       </c>
     </row>
   </sheetData>
@@ -1373,11 +1606,12 @@
     <hyperlink ref="F9" r:id="rId2"/>
     <hyperlink ref="F7" r:id="rId3"/>
     <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F12" r:id="rId5"/>
-    <hyperlink ref="F14" r:id="rId6"/>
-    <hyperlink ref="F20" r:id="rId7"/>
+    <hyperlink ref="F11" r:id="rId5"/>
+    <hyperlink ref="F15" r:id="rId6"/>
+    <hyperlink ref="F21" r:id="rId7"/>
+    <hyperlink ref="F62" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New helper in project
</commit_message>
<xml_diff>
--- a/Scheme/Smeta.xlsx
+++ b/Scheme/Smeta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Migrate to Quartus 18.1 Migrate to STM32Cube FW_F4 1.24 Loyouts update Cleanups
</commit_message>
<xml_diff>
--- a/Scheme/Smeta.xlsx
+++ b/Scheme/Smeta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
   <si>
     <t>Наименование</t>
   </si>
@@ -86,15 +86,9 @@
     <t>Диод 1N4148WS</t>
   </si>
   <si>
-    <t>Реле V23079A2003B301 12вольт 2 пер</t>
-  </si>
-  <si>
     <t>Плата УНЧ</t>
   </si>
   <si>
-    <t>Модуль PAM8403 ADJ УНЧ 2*3W 2,5-5V с регулятором</t>
-  </si>
-  <si>
     <t>Стабилизатор LM1117S-ADJ D2PAK</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>Конденсатор 1мкф</t>
   </si>
   <si>
-    <t>Корпус РЭА №15-9 200*165*65</t>
-  </si>
-  <si>
     <t>Плата УВЧ (Preamp)</t>
   </si>
   <si>
@@ -203,42 +194,21 @@
     <t>Штекер MIC 8pin</t>
   </si>
   <si>
-    <t>Кварц 12МГц HC-49US</t>
-  </si>
-  <si>
-    <t>Конденсатор 22пф</t>
-  </si>
-  <si>
     <t>Гнездо питания 5,5*2,1</t>
   </si>
   <si>
-    <t>Мембранная клавиатура 1*4</t>
-  </si>
-  <si>
-    <t>Диод Шоттки SR860 (SB860) DO-201 60V 8A</t>
-  </si>
-  <si>
-    <t>DC-DC 4,0-38V -&gt; 1,25-36V 5A LM2596S-ADJ понижающий</t>
-  </si>
-  <si>
     <t>Кнопка питания, с фиксацией PBS-16A 220М 1A</t>
   </si>
   <si>
     <t>Оптический энкодер 600 позиций на оборот</t>
   </si>
   <si>
-    <t>Гнездо SMA на плату</t>
-  </si>
-  <si>
     <t>Переключатель TX-RX</t>
   </si>
   <si>
     <t>Модуль реле 1-канальный 5В 10A 250V/реле</t>
   </si>
   <si>
-    <t>SMA-SMA патч корд 6,5"</t>
-  </si>
-  <si>
     <t>https://ru.aliexpress.com/item/100-NEW-Original-ADT4-6WT-ADT4-6-WT-ADT4-6WT-0-5-MHz-600-MHz-RF/32764096262.html</t>
   </si>
   <si>
@@ -257,18 +227,6 @@
     <t>Итого трансивер</t>
   </si>
   <si>
-    <t>https://ru.aliexpress.com/item/45W-3-28MHz-SSB-linear-Power-Amplifier-board-DIY-Kits-for-transceiver-Radio-HF-FM-CW/32808409970.html</t>
-  </si>
-  <si>
-    <t>Усилитель 45Вт</t>
-  </si>
-  <si>
-    <t>Радиатор HS183-100 50*100*16мм</t>
-  </si>
-  <si>
-    <t>Штекер SMA на кабель RG-174</t>
-  </si>
-  <si>
     <t>Кабель RG-178 50 Ом</t>
   </si>
   <si>
@@ -278,10 +236,34 @@
     <t>Динамическая головка TRI57N-A 1Вт 8Ом</t>
   </si>
   <si>
-    <t>Транзистор BC337 TO92 NPN</t>
-  </si>
-  <si>
-    <t>Транзистор C2078</t>
+    <t>LM1117-3.3</t>
+  </si>
+  <si>
+    <t>Ферритовая бусина</t>
+  </si>
+  <si>
+    <t>Штекер MMCX на кабель</t>
+  </si>
+  <si>
+    <t>Гнездо MMCX на плату</t>
+  </si>
+  <si>
+    <t>https://ru.aliexpress.com/item/YILIANDUO-10-MMCX-LMR100/32946181371.html</t>
+  </si>
+  <si>
+    <t>https://ru.aliexpress.com/item/5-MMCX-Jack/32892212454.html</t>
+  </si>
+  <si>
+    <t>LM7805</t>
+  </si>
+  <si>
+    <t>LM7812</t>
+  </si>
+  <si>
+    <t>https://ru.aliexpress.com/item/DF2-DC12V-12-DF2-8-12VDC/32854815553.html</t>
+  </si>
+  <si>
+    <t>Реле DF2-DC12V</t>
   </si>
 </sst>
 </file>
@@ -659,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F82"/>
+  <dimension ref="B2:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -687,7 +669,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -710,7 +692,7 @@
         <v>2278.73</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -724,7 +706,7 @@
         <v>182.11</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" ref="E5:E71" si="0">C5*D5</f>
+        <f t="shared" ref="E5:E74" si="0">C5*D5</f>
         <v>182.11</v>
       </c>
     </row>
@@ -748,7 +730,7 @@
         <v>707.81</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -766,7 +748,7 @@
         <v>479.67</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -784,7 +766,7 @@
         <v>714.68</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -807,199 +789,198 @@
         <v>933.21</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="7">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1236.95</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>1236.95</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D14" s="7">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
-      <c r="E13" s="7">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
-      </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
-        <v>1236.95</v>
-      </c>
-      <c r="E15" s="7">
-        <f t="shared" si="0"/>
-        <v>1236.95</v>
-      </c>
-      <c r="F15" s="10" t="s">
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>800</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="5">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
+        <v>67.5</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="0"/>
+        <v>67.5</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
         <f>5/10</f>
         <v>0.5</v>
       </c>
-      <c r="E16" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="E20" s="7">
+        <f>C20*D20</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="5">
         <v>2</v>
       </c>
-      <c r="D17" s="7">
-        <f>5/10</f>
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="D21" s="7">
+        <v>5</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E22" s="7">
         <f t="shared" si="0"/>
         <v>1.4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7">
-        <v>800</v>
-      </c>
-      <c r="E19" s="7">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7">
-        <v>67.5</v>
-      </c>
-      <c r="E21" s="7">
-        <f t="shared" si="0"/>
-        <v>67.5</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7">
-        <f>5/10</f>
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="7">
-        <f>C22*D22</f>
-        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C23" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="7">
-        <v>5</v>
+        <f>7/5</f>
+        <v>1.4</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C24" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D24" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
       <c r="E24" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
+        <f>C24*D24</f>
+        <v>8.3999999999999986</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -1007,36 +988,34 @@
         <v>32</v>
       </c>
       <c r="C25" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="7">
-        <f>7/5</f>
-        <v>1.4</v>
+        <v>6</v>
       </c>
       <c r="E25" s="7">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
+        <f>C25*D25</f>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C26" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D26" s="7">
-        <f>7/5</f>
-        <v>1.4</v>
+        <v>12</v>
       </c>
       <c r="E26" s="7">
         <f>C26*D26</f>
-        <v>5.6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>2</v>
@@ -1051,147 +1030,164 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
       </c>
       <c r="D28" s="7">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="E28" s="7">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <f t="shared" ref="E28:E29" si="1">C28*D28</f>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="5">
+        <v>2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>17</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7">
+        <f>73.3/5</f>
+        <v>14.66</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" si="0"/>
+        <v>14.66</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7">
+        <f>254.5/10</f>
+        <v>25.45</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="0"/>
+        <v>25.45</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="5">
-        <v>1</v>
-      </c>
-      <c r="D29" s="7">
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7">
         <f>665/5</f>
         <v>133</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E32" s="7">
         <f t="shared" si="0"/>
         <v>133</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="5">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7">
-        <v>145</v>
-      </c>
-      <c r="E31" s="7">
-        <f t="shared" si="0"/>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>16</v>
+      <c r="F32" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="5">
-        <v>1</v>
-      </c>
-      <c r="D33" s="7">
-        <v>170</v>
-      </c>
-      <c r="E33" s="7">
-        <f t="shared" si="0"/>
-        <v>170</v>
+      <c r="B33" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C34" s="5">
         <v>1</v>
       </c>
       <c r="D34" s="7">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E34" s="7">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="C36" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D36" s="7">
-        <f>7/5</f>
-        <v>1.4</v>
+        <v>19</v>
       </c>
       <c r="E36" s="7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="C37" s="5">
         <v>1</v>
       </c>
       <c r="D37" s="7">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E37" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C38" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="7">
         <v>12</v>
       </c>
       <c r="E38" s="7">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>C38*D38</f>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C39" s="5">
         <v>4</v>
@@ -1201,126 +1197,114 @@
         <v>1.4</v>
       </c>
       <c r="E39" s="7">
-        <f t="shared" si="0"/>
+        <f>C39*D39</f>
         <v>5.6</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="5">
-        <v>2</v>
-      </c>
-      <c r="D40" s="7">
+      <c r="B40" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="5">
+        <v>5</v>
+      </c>
+      <c r="D41" s="7">
         <f>7/5</f>
         <v>1.4</v>
       </c>
-      <c r="E40" s="7">
-        <f t="shared" si="0"/>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="5">
-        <v>2</v>
-      </c>
-      <c r="D41" s="7">
-        <v>0.9</v>
-      </c>
       <c r="E41" s="7">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C42" s="5">
         <v>1</v>
       </c>
       <c r="D42" s="7">
-        <f>5/10</f>
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="E42" s="7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C43" s="5">
         <v>1</v>
       </c>
       <c r="D43" s="7">
-        <f>5/10</f>
-        <v>0.5</v>
+        <v>12</v>
       </c>
       <c r="E43" s="7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C44" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D44" s="7">
-        <v>0.9</v>
+        <f>7/5</f>
+        <v>1.4</v>
       </c>
       <c r="E44" s="7">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C45" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" s="7">
-        <f>5/10</f>
-        <v>0.5</v>
+        <f>7/5</f>
+        <v>1.4</v>
       </c>
       <c r="E45" s="7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C46" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" s="7">
-        <f>5/10</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E46" s="7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C47" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D47" s="7">
         <f>5/10</f>
@@ -1328,486 +1312,454 @@
       </c>
       <c r="E47" s="7">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C48" s="5">
         <v>1</v>
       </c>
       <c r="D48" s="7">
-        <v>8</v>
+        <f>5/10</f>
+        <v>0.5</v>
       </c>
       <c r="E48" s="7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C49" s="5">
         <v>1</v>
       </c>
       <c r="D49" s="7">
-        <v>4</v>
+        <v>0.9</v>
       </c>
       <c r="E49" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" s="7">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+      <c r="D51" s="7">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="E51" s="7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="5">
+        <v>3</v>
+      </c>
+      <c r="D52" s="7">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="E52" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="5">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7">
+        <v>8</v>
+      </c>
+      <c r="E53" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
+      </c>
+      <c r="D54" s="7">
+        <v>4</v>
+      </c>
+      <c r="E54" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="5">
-        <v>1</v>
-      </c>
-      <c r="D50" s="7">
+      <c r="C55" s="5">
+        <v>1</v>
+      </c>
+      <c r="D55" s="7">
         <f>129.2/10</f>
         <v>12.919999999999998</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E55" s="7">
         <f t="shared" si="0"/>
         <v>12.919999999999998</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="5">
-        <v>2</v>
-      </c>
-      <c r="D51" s="7">
-        <v>11</v>
-      </c>
-      <c r="E51" s="7">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="5">
-        <v>4</v>
-      </c>
-      <c r="D52" s="7">
-        <v>6</v>
-      </c>
-      <c r="E52" s="7">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="5">
-        <v>1</v>
-      </c>
-      <c r="D53" s="7">
-        <v>150</v>
-      </c>
-      <c r="E53" s="7">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="5">
-        <v>1</v>
-      </c>
-      <c r="D54" s="7">
-        <v>4</v>
-      </c>
-      <c r="E54" s="7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" s="5">
-        <v>1</v>
-      </c>
-      <c r="D55" s="7">
-        <v>46</v>
-      </c>
-      <c r="E55" s="7">
-        <f t="shared" si="0"/>
-        <v>46</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="C56" s="5">
         <v>2</v>
       </c>
       <c r="D56" s="7">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="E56" s="7">
         <f t="shared" si="0"/>
-        <v>158</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
-        <v>68</v>
+      <c r="B57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="5">
+        <v>4</v>
+      </c>
+      <c r="D57" s="7">
+        <v>6</v>
+      </c>
+      <c r="E57" s="7">
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C58" s="5">
         <v>1</v>
       </c>
       <c r="D58" s="7">
-        <v>89</v>
+        <f>207/5</f>
+        <v>41.4</v>
       </c>
       <c r="E58" s="7">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>41.4</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="C59" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" s="7">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="E59" s="7">
         <f t="shared" si="0"/>
-        <v>158</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
-        <v>40</v>
+      <c r="B60" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" s="5">
+        <v>1</v>
+      </c>
+      <c r="D60" s="7">
+        <v>46</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="C61" s="5">
         <v>1</v>
       </c>
       <c r="D61" s="7">
-        <v>79</v>
+        <f>73.3/5</f>
+        <v>14.66</v>
       </c>
       <c r="E61" s="7">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <f t="shared" ref="E61:E62" si="2">C61*D61</f>
+        <v>14.66</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C62" s="5">
         <v>1</v>
       </c>
       <c r="D62" s="7">
-        <v>525</v>
+        <f>254.5/10</f>
+        <v>25.45</v>
       </c>
       <c r="E62" s="7">
-        <f t="shared" si="0"/>
-        <v>525</v>
+        <f t="shared" si="2"/>
+        <v>25.45</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="5">
-        <v>1</v>
-      </c>
-      <c r="D63" s="7">
-        <v>962</v>
-      </c>
-      <c r="E63" s="7">
-        <f t="shared" si="0"/>
-        <v>962</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>56</v>
+      <c r="B63" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C64" s="5">
         <v>1</v>
       </c>
       <c r="D64" s="7">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="E64" s="7">
         <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="F64" s="10"/>
+        <v>89</v>
+      </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="C65" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D65" s="7">
-        <v>45</v>
+        <f>73.3/5</f>
+        <v>14.66</v>
       </c>
       <c r="E65" s="7">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F65" s="10"/>
+        <v>29.32</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C66" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D66" s="7">
-        <v>27</v>
+        <f>254.5/10</f>
+        <v>25.45</v>
       </c>
       <c r="E66" s="7">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="F66" s="10"/>
+        <v>50.9</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C67" s="5">
-        <v>1</v>
-      </c>
-      <c r="D67" s="7">
-        <v>60</v>
-      </c>
-      <c r="E67" s="7">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="F67" s="10"/>
+      <c r="B67" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C68" s="5">
         <v>1</v>
       </c>
       <c r="D68" s="7">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="E68" s="7">
         <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="F68" s="10"/>
+        <v>79</v>
+      </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C69" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D69" s="7">
-        <v>67</v>
+        <v>962</v>
       </c>
       <c r="E69" s="7">
         <f t="shared" si="0"/>
-        <v>201</v>
-      </c>
-      <c r="F69" s="10"/>
+        <v>962</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C70" s="5">
         <v>1</v>
       </c>
       <c r="D70" s="7">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="E70" s="7">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="F70" s="10"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C71" s="5">
         <v>1</v>
       </c>
       <c r="D71" s="7">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E71" s="7">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F71" s="10"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>78</v>
+      <c r="B72" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C72" s="5">
         <v>1</v>
       </c>
       <c r="D72" s="7">
-        <v>963</v>
+        <v>27</v>
       </c>
       <c r="E72" s="7">
-        <f>C72*D72</f>
-        <v>963</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>77</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="F72" s="10"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C73" s="5">
         <v>1</v>
       </c>
       <c r="D73" s="7">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="E73" s="7">
-        <f>C73*D73</f>
-        <v>97</v>
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
       <c r="F73" s="10"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C74" s="5">
         <v>1</v>
       </c>
       <c r="D74" s="7">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="E74" s="7">
-        <f t="shared" ref="E74" si="1">C74*D74</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="F74" s="10"/>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+      <c r="D75" s="7">
         <v>85</v>
       </c>
-      <c r="C75" s="5">
-        <v>1</v>
-      </c>
-      <c r="D75" s="7">
-        <v>72</v>
-      </c>
       <c r="E75" s="7">
-        <f>C75*D75</f>
-        <v>72</v>
+        <f t="shared" ref="E75" si="3">C75*D75</f>
+        <v>85</v>
       </c>
       <c r="F75" s="10"/>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C76" s="5">
-        <v>1</v>
-      </c>
-      <c r="D76" s="7">
-        <v>89</v>
-      </c>
-      <c r="E76" s="7">
-        <f>C76*D76</f>
-        <v>89</v>
-      </c>
-      <c r="F76" s="10"/>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C77" s="5">
-        <v>2</v>
-      </c>
-      <c r="D77" s="7">
-        <v>79</v>
-      </c>
-      <c r="E77" s="7">
-        <f t="shared" ref="E77:E78" si="2">C77*D77</f>
-        <v>158</v>
-      </c>
-      <c r="F77" s="10"/>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C78" s="5">
-        <v>1</v>
-      </c>
-      <c r="D78" s="7">
-        <v>85</v>
-      </c>
-      <c r="E78" s="7">
-        <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="F78" s="10"/>
+      <c r="B76" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E76" s="8">
+        <f>SUM(E3:E75)</f>
+        <v>9543.119999999999</v>
+      </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E79" s="8">
-        <f>SUM(E3:E78)</f>
-        <v>12260.68</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="9"/>
+      <c r="B79" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1816,14 +1768,20 @@
     <hyperlink ref="F7" r:id="rId3"/>
     <hyperlink ref="F4" r:id="rId4"/>
     <hyperlink ref="F11" r:id="rId5"/>
-    <hyperlink ref="F15" r:id="rId6"/>
-    <hyperlink ref="F21" r:id="rId7"/>
-    <hyperlink ref="F63" r:id="rId8"/>
-    <hyperlink ref="F19" r:id="rId9"/>
-    <hyperlink ref="F29" r:id="rId10"/>
-    <hyperlink ref="F72" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId6"/>
+    <hyperlink ref="F19" r:id="rId7"/>
+    <hyperlink ref="F69" r:id="rId8"/>
+    <hyperlink ref="F17" r:id="rId9"/>
+    <hyperlink ref="F32" r:id="rId10"/>
+    <hyperlink ref="F31" r:id="rId11"/>
+    <hyperlink ref="F30" r:id="rId12"/>
+    <hyperlink ref="F58" r:id="rId13"/>
+    <hyperlink ref="F62" r:id="rId14"/>
+    <hyperlink ref="F61" r:id="rId15"/>
+    <hyperlink ref="F66" r:id="rId16"/>
+    <hyperlink ref="F65" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Layouts update Some cleanups
</commit_message>
<xml_diff>
--- a/Scheme/Smeta.xlsx
+++ b/Scheme/Smeta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Develop\Projects\UA3REO\Scheme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -257,13 +257,13 @@
     <t>LM7805</t>
   </si>
   <si>
-    <t>LM7812</t>
-  </si>
-  <si>
     <t>https://ru.aliexpress.com/item/DF2-DC12V-12-DF2-8-12VDC/32854815553.html</t>
   </si>
   <si>
     <t>Реле DF2-DC12V</t>
+  </si>
+  <si>
+    <t>Диод Шоттки SR860 (SB860) DO-201 60V 8A</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1142,17 +1144,17 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C36" s="5">
         <v>1</v>
       </c>
       <c r="D36" s="7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E36" s="7">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -1472,7 +1474,7 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C58" s="5">
         <v>1</v>
@@ -1486,7 +1488,7 @@
         <v>41.4</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
@@ -1755,7 +1757,7 @@
       </c>
       <c r="E76" s="8">
         <f>SUM(E3:E75)</f>
-        <v>9543.119999999999</v>
+        <v>9542.119999999999</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>